<commit_message>
update day 62 and 63
</commit_message>
<xml_diff>
--- a/_PowerPoints/2nd Semester/Unit 8 Bridge Building/B2 Projects/Summative Sheet.xlsx
+++ b/_PowerPoints/2nd Semester/Unit 8 Bridge Building/B2 Projects/Summative Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="55">
   <si>
     <t>Jordan B</t>
   </si>
@@ -737,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1049,16 +1049,22 @@
       <c r="E12" s="1">
         <v>4</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="G12" s="1" t="s">
         <v>49</v>
       </c>
       <c r="H12" s="1">
         <v>40</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="I12" s="1">
+        <v>4</v>
+      </c>
       <c r="J12" s="3"/>
-      <c r="K12" s="19"/>
+      <c r="K12" s="19">
+        <v>4</v>
+      </c>
       <c r="L12" s="8"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
@@ -1075,16 +1081,22 @@
       <c r="E13" s="1">
         <v>4</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="G13" s="1" t="s">
         <v>49</v>
       </c>
       <c r="H13" s="1">
         <v>40</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="I13" s="1">
+        <v>4</v>
+      </c>
       <c r="J13" s="3"/>
-      <c r="K13" s="19"/>
+      <c r="K13" s="19">
+        <v>4</v>
+      </c>
       <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
@@ -1101,16 +1113,22 @@
       <c r="E14" s="1">
         <v>4</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="G14" s="1" t="s">
         <v>49</v>
       </c>
       <c r="H14" s="1">
         <v>40</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="I14" s="1">
+        <v>4</v>
+      </c>
       <c r="J14" s="3"/>
-      <c r="K14" s="19"/>
+      <c r="K14" s="19">
+        <v>4</v>
+      </c>
       <c r="L14" s="8"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">

</xml_diff>